<commit_message>
fixing import data santri
</commit_message>
<xml_diff>
--- a/public/files/Format import data santri.xlsx
+++ b/public/files/Format import data santri.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
   <si>
     <t>nama</t>
   </si>
   <si>
-    <t>kelas_id</t>
-  </si>
-  <si>
-    <t>kamar_id</t>
+    <t>kode_kelas</t>
+  </si>
+  <si>
+    <t>kode_kamar</t>
   </si>
   <si>
     <t>no_induk</t>
@@ -91,6 +91,12 @@
     <t>Ahmad Muzayyin</t>
   </si>
   <si>
+    <t>WEZNC20300</t>
+  </si>
+  <si>
+    <t>QKUZQ10444</t>
+  </si>
+  <si>
     <t>Mandala Barat</t>
   </si>
   <si>
@@ -158,6 +164,9 @@
   </si>
   <si>
     <t>Moh. Wildan</t>
+  </si>
+  <si>
+    <t>ULKLN41341</t>
   </si>
   <si>
     <t>2012-03-17</t>
@@ -1127,12 +1136,14 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="9.375" style="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="10.875" customWidth="1"/>
@@ -1234,222 +1245,222 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
       </c>
       <c r="D2" s="1">
         <v>14450001</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N2" s="1">
         <v>15</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P2" s="1">
         <v>1999</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="X2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="1">
         <v>14450002</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1">
         <v>15</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P3" s="1">
         <v>1999</v>
       </c>
       <c r="Q3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="X3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
       </c>
       <c r="D4" s="1">
         <v>14450003</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N4" s="1">
         <v>15</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P4" s="1">
         <v>1999</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="X4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing field import data format
</commit_message>
<xml_diff>
--- a/public/files/Format import data santri.xlsx
+++ b/public/files/Format import data santri.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12435"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>nama</t>
   </si>
@@ -25,9 +25,6 @@
     <t>kode_kamar</t>
   </si>
   <si>
-    <t>no_induk</t>
-  </si>
-  <si>
     <t>dusun</t>
   </si>
   <si>
@@ -70,15 +67,9 @@
     <t>tahun_masuk</t>
   </si>
   <si>
-    <t>tahun_masuk_hijriyah</t>
-  </si>
-  <si>
     <t>tanggal_boyong</t>
   </si>
   <si>
-    <t>tanggal_boyong_hijriyah</t>
-  </si>
-  <si>
     <t>nama_ayah</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t>isi kode kamar</t>
   </si>
   <si>
-    <t>lanjutkan nomor induk di aplikasi</t>
-  </si>
-  <si>
     <t>diisi dusun</t>
   </si>
   <si>
@@ -139,13 +127,7 @@
     <t>2012-03-15</t>
   </si>
   <si>
-    <t>04-05-1434</t>
-  </si>
-  <si>
     <t>2017-03-15</t>
-  </si>
-  <si>
-    <t>02-10-1440</t>
   </si>
   <si>
     <t>diisi nama ayah</t>
@@ -160,10 +142,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -174,6 +156,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -182,8 +188,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +204,52 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,10 +264,17 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -221,21 +287,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -243,78 +294,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -327,13 +309,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,13 +405,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,19 +453,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,127 +483,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,6 +500,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -532,15 +523,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,20 +542,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,17 +583,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,148 +605,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -772,10 +754,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1100,10 +1082,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -1111,29 +1093,26 @@
     <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="2" max="2" width="13.625" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="10.625" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="19.75" customWidth="1"/>
-    <col min="11" max="11" width="17.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.25" style="2" customWidth="1"/>
-    <col min="13" max="13" width="29.875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" customWidth="1"/>
-    <col min="18" max="18" width="12.75" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.25" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.75" style="1" customWidth="1"/>
-    <col min="21" max="21" width="22.25" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.625" customWidth="1"/>
-    <col min="23" max="23" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="10.875" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="7" width="16.125" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="19.75" customWidth="1"/>
+    <col min="10" max="10" width="17.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="29.875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.75" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.625" customWidth="1"/>
+    <col min="20" max="20" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1122,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1161,118 +1140,100 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>39</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>